<commit_message>
feat: :zap: Adding more analysis on accountants at startups research
</commit_message>
<xml_diff>
--- a/research-in-acc-sciences/accountant-profile-in-startups/glossary_tech_manually_reviewed.xlsx
+++ b/research-in-acc-sciences/accountant-profile-in-startups/glossary_tech_manually_reviewed.xlsx
@@ -15,14 +15,14 @@
     <sheet name="glossary_tech_processed" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">glossary_tech_processed!$A$1:$H$481</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">glossary_tech_processed!$A$1:$I$481</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3853" uniqueCount="2624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3853" uniqueCount="2625">
   <si>
     <t>category_en</t>
   </si>
@@ -7894,6 +7894,9 @@
   </si>
   <si>
     <t xml:space="preserve">Microsoft Excel </t>
+  </si>
+  <si>
+    <t>excel</t>
   </si>
 </sst>
 </file>
@@ -11135,10 +11138,10 @@
         <v>2623</v>
       </c>
       <c r="G93" t="s">
-        <v>520</v>
+        <v>2624</v>
       </c>
       <c r="H93" t="s">
-        <v>521</v>
+        <v>2624</v>
       </c>
       <c r="I93" t="s">
         <v>2620</v>

</xml_diff>